<commit_message>
Update UI and XML to support same-name arguments (e.g. in Contact.Contact.* events)
</commit_message>
<xml_diff>
--- a/helpers/KAIROS_Annotation_Tagset_Phase_1_V2.0_argsplit.xlsx
+++ b/helpers/KAIROS_Annotation_Tagset_Phase_1_V2.0_argsplit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anton/kairos/schema-ui/helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61856A6E-350C-C84E-92E5-F854FFC3DB47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D8B0B7-F35A-5048-B035-47DCA731FE58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="1270">
   <si>
     <t>AnnotIndexID</t>
   </si>
@@ -3825,7 +3825,13 @@
     <t>&lt;arg1&gt; bought, sold, or traded &lt;arg3&gt; | to &lt;arg2&gt; | in exchange for &lt;arg4&gt; | for the benefit of &lt;arg5&gt; | at &lt;arg6&gt; place</t>
   </si>
   <si>
-    <t>Participant2</t>
+    <t>&lt;arg1&gt; met face-to-face | with &lt;arg2&gt; | about &lt;arg3&gt; topic | at &lt;arg4&gt; place</t>
+  </si>
+  <si>
+    <t>&lt;arg1&gt; communicated remotely | with &lt;arg2&gt; | about &lt;arg4&gt; topic | using &lt;arg3&gt; | at &lt;arg5&gt; place</t>
+  </si>
+  <si>
+    <t>&lt;arg1&gt; communicated | with &lt;arg2&gt; | about &lt;arg3&gt; topic | at &lt;arg4&gt; place | (document does not specify in person or not, or one-way or not)</t>
   </si>
 </sst>
 </file>
@@ -4171,9 +4177,9 @@
   </sheetPr>
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5536,7 +5542,7 @@
         <v>243</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>1228</v>
+        <v>1268</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>244</v>
@@ -5548,7 +5554,7 @@
         <v>37</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>1267</v>
+        <v>244</v>
       </c>
       <c r="N18" s="10" t="s">
         <v>246</v>
@@ -5615,7 +5621,7 @@
         <v>253</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>1229</v>
+        <v>1267</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>244</v>
@@ -5627,7 +5633,7 @@
         <v>37</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>1267</v>
+        <v>244</v>
       </c>
       <c r="N19" s="10" t="s">
         <v>255</v>
@@ -5688,7 +5694,7 @@
         <v>259</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>1230</v>
+        <v>1269</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>244</v>
@@ -5700,7 +5706,7 @@
         <v>37</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>1267</v>
+        <v>244</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>261</v>

</xml_diff>